<commit_message>
updated plot buying costs
</commit_message>
<xml_diff>
--- a/reward calculations.xlsx
+++ b/reward calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlf\go\src\github.com\CarlFlo\DiscordMoneyBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD15ADF6-F3D2-433E-845C-B16D2E1534A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A406EFE-F098-4051-83A2-33CF8498FEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19560" yWindow="0" windowWidth="18435" windowHeight="15015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>#</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>Seed price</t>
+  </si>
+  <si>
+    <t>Farmplot price</t>
+  </si>
+  <si>
+    <t>Base farmplot price</t>
+  </si>
+  <si>
+    <t>Plot price multi</t>
   </si>
 </sst>
 </file>
@@ -373,7 +382,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +391,8 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -399,6 +409,9 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
       <c r="O1" t="s">
         <v>3</v>
       </c>
@@ -416,6 +429,10 @@
       <c r="D2">
         <f>(C2-$K$2)/B2</f>
         <v>2.5</v>
+      </c>
+      <c r="F2">
+        <f>ROUNDDOWN($K$3*$K$4^(A2-1),0)</f>
+        <v>5000</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
@@ -442,13 +459,23 @@
         <f t="shared" ref="D3:D16" si="0">(C3-$K$2)/B3</f>
         <v>2.3333333333333335</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="1">ROUNDDOWN($K$3*$K$4^(A3-1),0)</f>
+        <v>7500</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <v>5000</v>
+      </c>
       <c r="O3">
         <v>1200</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A15" si="1">A3+1</f>
+        <f t="shared" ref="A4:A15" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -461,13 +488,23 @@
         <f t="shared" si="0"/>
         <v>2.0833333333333335</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>11250</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>1.5</v>
+      </c>
       <c r="O4">
         <v>1750</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -481,13 +518,17 @@
         <f t="shared" si="0"/>
         <v>1.8333333333333333</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>16875</v>
+      </c>
       <c r="O5">
         <v>3800</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="B6">
@@ -501,13 +542,17 @@
         <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>25312</v>
+      </c>
       <c r="O6">
         <v>6800</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="B7">
@@ -521,13 +566,17 @@
         <f t="shared" si="0"/>
         <v>1.625</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>37968</v>
+      </c>
       <c r="O7">
         <v>12200</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -541,13 +590,17 @@
         <f t="shared" si="0"/>
         <v>1.5625</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>56953</v>
+      </c>
       <c r="O8">
         <v>23000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -560,6 +613,10 @@
       <c r="D9">
         <f t="shared" si="0"/>
         <v>1.4756944444444444</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>85429</v>
       </c>
       <c r="O9">
         <v>43000</v>
@@ -581,13 +638,17 @@
         <f t="shared" si="0"/>
         <v>1.4236111111111112</v>
       </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>128144</v>
+      </c>
       <c r="O10">
         <v>62000</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="B11">
@@ -607,7 +668,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="B12">
@@ -627,7 +688,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="B13">
@@ -647,7 +708,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B14">
@@ -667,7 +728,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B15">

</xml_diff>